<commit_message>
Added more backlog items
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>What</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>Vinit</t>
+  </si>
+  <si>
+    <t>Add Metadata files path as configurable path</t>
+  </si>
+  <si>
+    <t>Add SKIP UI/Page generation to build and only build UI code</t>
+  </si>
+  <si>
+    <t>Update navigation component of UI</t>
   </si>
 </sst>
 </file>
@@ -108,8 +117,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:D7"/>
   <tableColumns count="4">
     <tableColumn id="1" name="#"/>
     <tableColumn id="2" name="What"/>
@@ -407,16 +416,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D7" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -465,6 +474,25 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>